<commit_message>
Added loading of fixed grids
</commit_message>
<xml_diff>
--- a/ExcelBot.Runtime/strategy.xlsx
+++ b/ExcelBot.Runtime/strategy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\prive\infinibattle-2023-excel-bot\ExcelBot.Runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AFEC48-B7FC-4642-9D44-2FEBB333CC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F5C237-56B5-466D-8A24-AE1F865B6ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{384E99EF-41B3-4078-AF7F-40BB6BDCDBD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{384E99EF-41B3-4078-AF7F-40BB6BDCDBD9}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelStrategie" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Flag</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>Miner</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Marshal</t>
@@ -222,7 +219,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCECFF"/>
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -275,9 +272,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -288,6 +282,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -674,7 +671,7 @@
   <dimension ref="B2:AV36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="AT26" sqref="AT26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,62 +686,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:48" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="M2" s="9" t="s">
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="M2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="X2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AI2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AT2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AI2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="9"/>
-      <c r="AP2" s="9"/>
-      <c r="AQ2" s="9"/>
-      <c r="AR2" s="9"/>
-      <c r="AT2" s="8" t="s">
+      <c r="AU2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AU2" s="7" t="s">
+      <c r="AV2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="AV2" s="7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -868,14 +865,14 @@
       <c r="AR3" s="3">
         <v>0</v>
       </c>
-      <c r="AT3" s="6">
+      <c r="AT3" s="5">
         <v>25</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1003,10 +1000,10 @@
         <v>95</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1134,10 +1131,10 @@
         <v>20</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1265,176 +1262,112 @@
         <v>98</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
-      <c r="AO7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AO7" s="9"/>
+      <c r="AP7" s="9"/>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
       <c r="AT7" s="2">
         <v>5</v>
       </c>
       <c r="AU7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AV7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
-      <c r="AK8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
       <c r="AM8" s="3"/>
       <c r="AN8" s="3"/>
-      <c r="AO8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP8" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AO8" s="9"/>
+      <c r="AP8" s="9"/>
       <c r="AQ8" s="3"/>
       <c r="AR8" s="3"/>
       <c r="AT8" s="2">
         <v>75</v>
       </c>
       <c r="AU8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AV8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1606,54 +1539,54 @@
       <c r="AR12" s="3"/>
     </row>
     <row r="14" spans="2:48" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="M14" s="9" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="M14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="X14" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y14" s="9"/>
-      <c r="Z14" s="9"/>
-      <c r="AA14" s="9"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
-      <c r="AF14" s="9"/>
-      <c r="AG14" s="9"/>
-      <c r="AI14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ14" s="9"/>
-      <c r="AK14" s="9"/>
-      <c r="AL14" s="9"/>
-      <c r="AM14" s="9"/>
-      <c r="AN14" s="9"/>
-      <c r="AO14" s="9"/>
-      <c r="AP14" s="9"/>
-      <c r="AQ14" s="9"/>
-      <c r="AR14" s="9"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="X14" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AI14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="8"/>
+      <c r="AQ14" s="8"/>
+      <c r="AR14" s="8"/>
     </row>
     <row r="15" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -2146,148 +2079,84 @@
     <row r="19" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
-      <c r="AD19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
-      <c r="AK19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
       <c r="AM19" s="3"/>
       <c r="AN19" s="3"/>
-      <c r="AO19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP19" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AO19" s="9"/>
+      <c r="AP19" s="9"/>
       <c r="AQ19" s="3"/>
       <c r="AR19" s="3"/>
     </row>
     <row r="20" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
-      <c r="S20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
-      <c r="AD20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="3"/>
-      <c r="AK20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
       <c r="AM20" s="3"/>
       <c r="AN20" s="3"/>
-      <c r="AO20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP20" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AO20" s="9"/>
+      <c r="AP20" s="9"/>
       <c r="AQ20" s="3"/>
       <c r="AR20" s="3"/>
     </row>
@@ -2460,61 +2329,61 @@
       <c r="AR24" s="3"/>
     </row>
     <row r="26" spans="2:44" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="M26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="X26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="8"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
+      <c r="AI26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="M26" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
-      <c r="X26" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y26" s="9"/>
-      <c r="Z26" s="9"/>
-      <c r="AA26" s="9"/>
-      <c r="AB26" s="9"/>
-      <c r="AC26" s="9"/>
-      <c r="AD26" s="9"/>
-      <c r="AE26" s="9"/>
-      <c r="AF26" s="9"/>
-      <c r="AG26" s="9"/>
-      <c r="AI26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AJ26" s="9"/>
-      <c r="AK26" s="9"/>
-      <c r="AL26" s="9"/>
-      <c r="AM26" s="9"/>
-      <c r="AN26" s="9"/>
-      <c r="AO26" s="9"/>
-      <c r="AP26" s="9"/>
-      <c r="AQ26" s="9"/>
-      <c r="AR26" s="9"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8"/>
+      <c r="AN26" s="8"/>
+      <c r="AO26" s="8"/>
+      <c r="AP26" s="8"/>
+      <c r="AQ26" s="8"/>
+      <c r="AR26" s="8"/>
     </row>
     <row r="27" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2557,10 +2426,10 @@
     </row>
     <row r="28" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -2603,10 +2472,10 @@
     </row>
     <row r="29" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2649,10 +2518,10 @@
     </row>
     <row r="30" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2664,28 +2533,28 @@
       <c r="K30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q30" s="3" t="s">
+      <c r="R30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R30" s="3" t="s">
+      <c r="S30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="S30" s="3" t="s">
+      <c r="T30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="T30" s="3" t="s">
+      <c r="U30" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="U30" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="V30" s="3"/>
       <c r="X30" s="3"/>
@@ -2712,148 +2581,84 @@
     <row r="31" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
-      <c r="Z31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
-      <c r="AD31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
-      <c r="AK31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AK31" s="9"/>
+      <c r="AL31" s="9"/>
       <c r="AM31" s="3"/>
       <c r="AN31" s="3"/>
-      <c r="AO31" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP31" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AO31" s="9"/>
+      <c r="AP31" s="9"/>
       <c r="AQ31" s="3"/>
       <c r="AR31" s="3"/>
     </row>
     <row r="32" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="T32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
-      <c r="Z32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
-      <c r="AD32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="3"/>
-      <c r="AK32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AK32" s="9"/>
+      <c r="AL32" s="9"/>
       <c r="AM32" s="3"/>
       <c r="AN32" s="3"/>
-      <c r="AO32" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP32" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="AO32" s="9"/>
+      <c r="AP32" s="9"/>
       <c r="AQ32" s="3"/>
       <c r="AR32" s="3"/>
     </row>

</xml_diff>

<commit_message>
Add fixed starting positions features
</commit_message>
<xml_diff>
--- a/ExcelBot.Runtime/strategy.xlsx
+++ b/ExcelBot.Runtime/strategy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\prive\infinibattle-2023-excel-bot\ExcelBot.Runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F5C237-56B5-466D-8A24-AE1F865B6ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1627640D-D696-4AE4-8482-697B489BBE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{384E99EF-41B3-4078-AF7F-40BB6BDCDBD9}"/>
   </bookViews>
@@ -60,21 +60,6 @@
     <t>Beschrijving</t>
   </si>
   <si>
-    <t>Clustering</t>
-  </si>
-  <si>
-    <t>BombFlagCombo</t>
-  </si>
-  <si>
-    <t>Secrecy</t>
-  </si>
-  <si>
-    <t>AgressivenessFactor</t>
-  </si>
-  <si>
-    <t>ReconnaissanceFactor</t>
-  </si>
-  <si>
     <t>Startpositie: hoe sterk de stukken in een cluster (vs. meer verspreid) starten.</t>
   </si>
   <si>
@@ -82,6 +67,45 @@
   </si>
   <si>
     <t>Actie: mate dat de bot geheim probeert te houden welke stukken kunnen bewegen.</t>
+  </si>
+  <si>
+    <t>Fixed Start 1</t>
+  </si>
+  <si>
+    <t>Fixed Start 4</t>
+  </si>
+  <si>
+    <t>Fixed Start 3</t>
+  </si>
+  <si>
+    <t>Fixed Start 2</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>Gebruik Fixed Start</t>
+  </si>
+  <si>
+    <t>Percentage kans dat een fixed startpositie (onderaan de sheet) gebruikt zal worden.</t>
   </si>
   <si>
     <r>
@@ -91,7 +115,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -101,7 +125,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -117,7 +141,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -127,7 +151,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -136,59 +160,27 @@
     </r>
   </si>
   <si>
-    <t>Startpositie: percentage kans dat een fixed startpositie gekozen wordt.</t>
-  </si>
-  <si>
-    <t>FixedStartPosition</t>
-  </si>
-  <si>
-    <t>Fixed Start 1</t>
-  </si>
-  <si>
-    <t>Fixed Start 4</t>
-  </si>
-  <si>
-    <t>Fixed Start 3</t>
-  </si>
-  <si>
-    <t>Fixed Start 2</t>
-  </si>
-  <si>
-    <t>FL</t>
-  </si>
-  <si>
-    <t>BO</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>GE</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>MI</t>
-  </si>
-  <si>
-    <t>SC</t>
+    <t>Clustering TODO</t>
+  </si>
+  <si>
+    <t>BombFlagCombo TODO</t>
+  </si>
+  <si>
+    <t>Secrecy TODO</t>
+  </si>
+  <si>
+    <t>AgressivenessFactor TODO</t>
+  </si>
+  <si>
+    <t>ReconnaissanceFactor TODO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,6 +191,21 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -271,21 +278,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,7 +681,7 @@
   <dimension ref="B2:AV36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AT26" sqref="AT26"/>
+      <selection activeCell="AT2" sqref="AT2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,59 +691,59 @@
     <col min="24" max="33" width="4.28515625" style="2" customWidth="1"/>
     <col min="35" max="44" width="4.28515625" style="2" customWidth="1"/>
     <col min="46" max="46" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="81.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:48" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="M2" s="8" t="s">
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="M2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="X2" s="8" t="s">
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="X2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AI2" s="8" t="s">
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AI2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="9"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
       <c r="AT2" s="7" t="s">
         <v>8</v>
       </c>
@@ -868,11 +878,11 @@
       <c r="AT3" s="5">
         <v>25</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AU3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AV3" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -999,11 +1009,11 @@
       <c r="AT4" s="2">
         <v>95</v>
       </c>
-      <c r="AU4" s="1" t="s">
+      <c r="AU4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AV4" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="AV4" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,13 +1138,13 @@
         <v>0</v>
       </c>
       <c r="AT5" s="2">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1261,113 +1271,113 @@
       <c r="AT6" s="2">
         <v>98</v>
       </c>
-      <c r="AU6" s="1" t="s">
+      <c r="AU6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AV6" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="AV6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="9"/>
-      <c r="AA7" s="9"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
-      <c r="AK7" s="9"/>
-      <c r="AL7" s="9"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
-      <c r="AO7" s="9"/>
-      <c r="AP7" s="9"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="8"/>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
       <c r="AT7" s="2">
         <v>5</v>
       </c>
-      <c r="AU7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV7" s="1" t="s">
-        <v>19</v>
+      <c r="AU7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV7" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="9"/>
-      <c r="AA8" s="9"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
-      <c r="AK8" s="9"/>
-      <c r="AL8" s="9"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
       <c r="AM8" s="3"/>
       <c r="AN8" s="3"/>
-      <c r="AO8" s="9"/>
-      <c r="AP8" s="9"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
       <c r="AQ8" s="3"/>
       <c r="AR8" s="3"/>
       <c r="AT8" s="2">
         <v>75</v>
       </c>
-      <c r="AU8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AV8" s="1" t="s">
-        <v>20</v>
+      <c r="AU8" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV8" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1539,54 +1549,54 @@
       <c r="AR12" s="3"/>
     </row>
     <row r="14" spans="2:48" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="M14" s="8" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="M14" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="X14" s="8" t="s">
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="X14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="8"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AI14" s="8" t="s">
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AI14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="8"/>
-      <c r="AO14" s="8"/>
-      <c r="AP14" s="8"/>
-      <c r="AQ14" s="8"/>
-      <c r="AR14" s="8"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
+      <c r="AN14" s="9"/>
+      <c r="AO14" s="9"/>
+      <c r="AP14" s="9"/>
+      <c r="AQ14" s="9"/>
+      <c r="AR14" s="9"/>
     </row>
     <row r="15" spans="2:48" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
@@ -2079,84 +2089,84 @@
     <row r="19" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
-      <c r="Z19" s="9"/>
-      <c r="AA19" s="9"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
       <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
       <c r="AI19" s="3"/>
       <c r="AJ19" s="3"/>
-      <c r="AK19" s="9"/>
-      <c r="AL19" s="9"/>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
       <c r="AM19" s="3"/>
       <c r="AN19" s="3"/>
-      <c r="AO19" s="9"/>
-      <c r="AP19" s="9"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
       <c r="AQ19" s="3"/>
       <c r="AR19" s="3"/>
     </row>
     <row r="20" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
       <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="X20" s="3"/>
       <c r="Y20" s="3"/>
-      <c r="Z20" s="9"/>
-      <c r="AA20" s="9"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="9"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
       <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AI20" s="3"/>
       <c r="AJ20" s="3"/>
-      <c r="AK20" s="9"/>
-      <c r="AL20" s="9"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
       <c r="AM20" s="3"/>
       <c r="AN20" s="3"/>
-      <c r="AO20" s="9"/>
-      <c r="AP20" s="9"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
       <c r="AQ20" s="3"/>
       <c r="AR20" s="3"/>
     </row>
@@ -2329,61 +2339,61 @@
       <c r="AR24" s="3"/>
     </row>
     <row r="26" spans="2:44" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="M26" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="X26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8"/>
-      <c r="AB26" s="8"/>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="8"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="8"/>
-      <c r="AI26" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ26" s="8"/>
-      <c r="AK26" s="8"/>
-      <c r="AL26" s="8"/>
-      <c r="AM26" s="8"/>
-      <c r="AN26" s="8"/>
-      <c r="AO26" s="8"/>
-      <c r="AP26" s="8"/>
-      <c r="AQ26" s="8"/>
-      <c r="AR26" s="8"/>
+      <c r="B26" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="M26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="X26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y26" s="9"/>
+      <c r="Z26" s="9"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AI26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="9"/>
+      <c r="AL26" s="9"/>
+      <c r="AM26" s="9"/>
+      <c r="AN26" s="9"/>
+      <c r="AO26" s="9"/>
+      <c r="AP26" s="9"/>
+      <c r="AQ26" s="9"/>
+      <c r="AR26" s="9"/>
     </row>
     <row r="27" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -2426,10 +2436,10 @@
     </row>
     <row r="28" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -2472,10 +2482,10 @@
     </row>
     <row r="29" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2518,10 +2528,10 @@
     </row>
     <row r="30" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2533,28 +2543,28 @@
       <c r="K30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="T30" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="U30" s="3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="V30" s="3"/>
       <c r="X30" s="3"/>
@@ -2581,84 +2591,84 @@
     <row r="31" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="3"/>
-      <c r="Z31" s="9"/>
-      <c r="AA31" s="9"/>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="8"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="9"/>
+      <c r="AD31" s="8"/>
+      <c r="AE31" s="8"/>
       <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
       <c r="AI31" s="3"/>
       <c r="AJ31" s="3"/>
-      <c r="AK31" s="9"/>
-      <c r="AL31" s="9"/>
+      <c r="AK31" s="8"/>
+      <c r="AL31" s="8"/>
       <c r="AM31" s="3"/>
       <c r="AN31" s="3"/>
-      <c r="AO31" s="9"/>
-      <c r="AP31" s="9"/>
+      <c r="AO31" s="8"/>
+      <c r="AP31" s="8"/>
       <c r="AQ31" s="3"/>
       <c r="AR31" s="3"/>
     </row>
     <row r="32" spans="2:44" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
       <c r="Q32" s="3"/>
       <c r="R32" s="3"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="3"/>
-      <c r="Z32" s="9"/>
-      <c r="AA32" s="9"/>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="8"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="9"/>
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="8"/>
       <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
       <c r="AI32" s="3"/>
       <c r="AJ32" s="3"/>
-      <c r="AK32" s="9"/>
-      <c r="AL32" s="9"/>
+      <c r="AK32" s="8"/>
+      <c r="AL32" s="8"/>
       <c r="AM32" s="3"/>
       <c r="AN32" s="3"/>
-      <c r="AO32" s="9"/>
-      <c r="AP32" s="9"/>
+      <c r="AO32" s="8"/>
+      <c r="AP32" s="8"/>
       <c r="AQ32" s="3"/>
       <c r="AR32" s="3"/>
     </row>

</xml_diff>